<commit_message>
Refine master data and add "Review Data"
</commit_message>
<xml_diff>
--- a/SpatialData/Strata_Volumes.xlsx
+++ b/SpatialData/Strata_Volumes.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\40545\Documents\GitHub\pelagicsurveys\SpatialData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{927CB8B4-5057-403F-A603-4B89A8C01657}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3CBB28C-FF20-4FB9-8D36-D43119A93865}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{80167769-BE09-4605-8E6B-D935EEDF2BE9}"/>
+    <workbookView xWindow="39660" yWindow="2190" windowWidth="13830" windowHeight="7170" xr2:uid="{80167769-BE09-4605-8E6B-D935EEDF2BE9}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -132,25 +132,25 @@
     <t>Grant Line Canal and Old River</t>
   </si>
   <si>
-    <t>Total (m³)</t>
-  </si>
-  <si>
-    <t>&gt;10m (m³)</t>
-  </si>
-  <si>
-    <t>8m-10m (m³)</t>
-  </si>
-  <si>
-    <t>6m-8m (m³)</t>
-  </si>
-  <si>
-    <t>4m-6m (m³)</t>
-  </si>
-  <si>
-    <t>2m-4m (m³)</t>
-  </si>
-  <si>
-    <t>&lt;2m (m³)</t>
+    <t>&lt;2m (km³)</t>
+  </si>
+  <si>
+    <t>2m-4m (km³)</t>
+  </si>
+  <si>
+    <t>4m-6m (km³)</t>
+  </si>
+  <si>
+    <t>6m-8m (km³)</t>
+  </si>
+  <si>
+    <t>8m-10m (km³)</t>
+  </si>
+  <si>
+    <t>&gt;10m (km³)</t>
+  </si>
+  <si>
+    <t>Total (km³)</t>
   </si>
 </sst>
 </file>
@@ -579,10 +579,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2E98462B-185A-40C8-B8AE-371C95AABD43}">
-  <dimension ref="A1:K32"/>
+  <dimension ref="A1:J32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H25" sqref="H25"/>
+      <selection activeCell="A2" sqref="A2:J31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -592,7 +592,7 @@
     <col min="4" max="16384" width="16.109375" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -603,28 +603,28 @@
         <v>2</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="G1" s="3" t="s">
         <v>36</v>
       </c>
       <c r="H1" s="3" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="I1" s="3" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="J1" s="3" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
         <v>3</v>
       </c>
@@ -655,12 +655,8 @@
       <c r="J2" s="14">
         <v>397.89</v>
       </c>
-      <c r="K2" s="14">
-        <f>B2*C2</f>
-        <v>397.88652508863993</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="s">
         <v>4</v>
       </c>
@@ -691,12 +687,8 @@
       <c r="J3" s="14">
         <v>242.23000000000002</v>
       </c>
-      <c r="K3" s="14">
-        <f t="shared" ref="K3:K31" si="0">B3*C3</f>
-        <v>242.23555678113999</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4" s="4" t="s">
         <v>5</v>
       </c>
@@ -727,12 +719,8 @@
       <c r="J4" s="14">
         <v>38.880000000000003</v>
       </c>
-      <c r="K4" s="14">
-        <f t="shared" si="0"/>
-        <v>38.886565610985002</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" s="9" customFormat="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="5" spans="1:10" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A5" s="7" t="s">
         <v>6</v>
       </c>
@@ -763,12 +751,8 @@
       <c r="J5" s="14">
         <v>1.1000000000000001</v>
       </c>
-      <c r="K5" s="14">
-        <f t="shared" si="0"/>
-        <v>1.1000988675157604</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A6" s="4" t="s">
         <v>7</v>
       </c>
@@ -799,12 +783,8 @@
       <c r="J6" s="14">
         <v>229.61</v>
       </c>
-      <c r="K6" s="14">
-        <f t="shared" si="0"/>
-        <v>229.59906387016076</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A7" s="4" t="s">
         <v>8</v>
       </c>
@@ -835,12 +815,8 @@
       <c r="J7" s="14">
         <v>200.10000000000002</v>
       </c>
-      <c r="K7" s="14">
-        <f t="shared" si="0"/>
-        <v>200.10324907866931</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A8" s="4" t="s">
         <v>9</v>
       </c>
@@ -871,12 +847,8 @@
       <c r="J8" s="14">
         <v>222.83</v>
       </c>
-      <c r="K8" s="14">
-        <f t="shared" si="0"/>
-        <v>222.81013606272001</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A9" s="4" t="s">
         <v>10</v>
       </c>
@@ -907,12 +879,8 @@
       <c r="J9" s="14">
         <v>45.13</v>
       </c>
-      <c r="K9" s="14">
-        <f t="shared" si="0"/>
-        <v>45.139848251066987</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A10" s="4" t="s">
         <v>11</v>
       </c>
@@ -943,12 +911,8 @@
       <c r="J10" s="14">
         <v>75.150000000000006</v>
       </c>
-      <c r="K10" s="14">
-        <f t="shared" si="0"/>
-        <v>75.13546243595033</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A11" s="4" t="s">
         <v>12</v>
       </c>
@@ -979,12 +943,8 @@
       <c r="J11" s="14">
         <v>162.45999999999998</v>
       </c>
-      <c r="K11" s="14">
-        <f t="shared" si="0"/>
-        <v>162.45718939116477</v>
-      </c>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A12" s="4" t="s">
         <v>13</v>
       </c>
@@ -1015,12 +975,8 @@
       <c r="J12" s="14">
         <v>85.500000000000014</v>
       </c>
-      <c r="K12" s="14">
-        <f t="shared" si="0"/>
-        <v>85.497291862602992</v>
-      </c>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A13" s="4" t="s">
         <v>14</v>
       </c>
@@ -1051,12 +1007,8 @@
       <c r="J13" s="14">
         <v>17.610000000000003</v>
       </c>
-      <c r="K13" s="14">
-        <f t="shared" si="0"/>
-        <v>17.601630470786997</v>
-      </c>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A14" s="4" t="s">
         <v>15</v>
       </c>
@@ -1087,12 +1039,8 @@
       <c r="J14" s="14">
         <v>30.099999999999998</v>
       </c>
-      <c r="K14" s="14">
-        <f t="shared" si="0"/>
-        <v>30.106128265174998</v>
-      </c>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A15" s="4" t="s">
         <v>16</v>
       </c>
@@ -1123,12 +1071,8 @@
       <c r="J15" s="14">
         <v>53.8</v>
       </c>
-      <c r="K15" s="14">
-        <f t="shared" si="0"/>
-        <v>53.80394974220718</v>
-      </c>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A16" s="4" t="s">
         <v>17</v>
       </c>
@@ -1159,12 +1103,8 @@
       <c r="J16" s="14">
         <v>40.78</v>
       </c>
-      <c r="K16" s="14">
-        <f t="shared" si="0"/>
-        <v>40.779872195249141</v>
-      </c>
-    </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A17" s="4" t="s">
         <v>18</v>
       </c>
@@ -1195,12 +1135,8 @@
       <c r="J17" s="14">
         <v>80.38</v>
       </c>
-      <c r="K17" s="14">
-        <f t="shared" si="0"/>
-        <v>80.379167758067837</v>
-      </c>
-    </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A18" s="4" t="s">
         <v>19</v>
       </c>
@@ -1231,12 +1167,8 @@
       <c r="J18" s="14">
         <v>74.75</v>
       </c>
-      <c r="K18" s="14">
-        <f t="shared" si="0"/>
-        <v>74.750337445228993</v>
-      </c>
-    </row>
-    <row r="19" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="19" spans="1:10" s="12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A19" s="10" t="s">
         <v>20</v>
       </c>
@@ -1267,12 +1199,8 @@
       <c r="J19" s="14">
         <v>2.8599999999999994</v>
       </c>
-      <c r="K19" s="14">
-        <f t="shared" si="0"/>
-        <v>2.862810602376229</v>
-      </c>
-    </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A20" s="4" t="s">
         <v>21</v>
       </c>
@@ -1303,12 +1231,8 @@
       <c r="J20" s="14">
         <v>155.41000000000003</v>
       </c>
-      <c r="K20" s="14">
-        <f t="shared" si="0"/>
-        <v>155.41392297639001</v>
-      </c>
-    </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A21" s="4" t="s">
         <v>22</v>
       </c>
@@ -1339,12 +1263,8 @@
       <c r="J21" s="14">
         <v>49.470000000000006</v>
       </c>
-      <c r="K21" s="14">
-        <f t="shared" si="0"/>
-        <v>49.468440620176004</v>
-      </c>
-    </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A22" s="4" t="s">
         <v>23</v>
       </c>
@@ -1375,12 +1295,8 @@
       <c r="J22" s="14">
         <v>81.110000000000014</v>
       </c>
-      <c r="K22" s="14">
-        <f t="shared" si="0"/>
-        <v>81.112160358886996</v>
-      </c>
-    </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.3">
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A23" s="4" t="s">
         <v>24</v>
       </c>
@@ -1411,12 +1327,8 @@
       <c r="J23" s="14">
         <v>27.52</v>
       </c>
-      <c r="K23" s="14">
-        <f t="shared" si="0"/>
-        <v>27.513443255890998</v>
-      </c>
-    </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.3">
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A24" s="4" t="s">
         <v>25</v>
       </c>
@@ -1447,12 +1359,8 @@
       <c r="J24" s="14">
         <v>49.16</v>
       </c>
-      <c r="K24" s="14">
-        <f t="shared" si="0"/>
-        <v>49.152733341868988</v>
-      </c>
-    </row>
-    <row r="25" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="25" spans="1:10" s="12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A25" s="10" t="s">
         <v>26</v>
       </c>
@@ -1483,12 +1391,8 @@
       <c r="J25" s="14">
         <v>3.9299999999999997</v>
       </c>
-      <c r="K25" s="14">
-        <f t="shared" si="0"/>
-        <v>3.9337528764680001</v>
-      </c>
-    </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.3">
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A26" s="4" t="s">
         <v>27</v>
       </c>
@@ -1519,12 +1423,8 @@
       <c r="J26" s="14">
         <v>13.76</v>
       </c>
-      <c r="K26" s="14">
-        <f t="shared" si="0"/>
-        <v>13.766613054081999</v>
-      </c>
-    </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.3">
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A27" s="4" t="s">
         <v>28</v>
       </c>
@@ -1555,12 +1455,8 @@
       <c r="J27" s="14">
         <v>49.95</v>
       </c>
-      <c r="K27" s="14">
-        <f t="shared" si="0"/>
-        <v>49.948920785124997</v>
-      </c>
-    </row>
-    <row r="28" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="28" spans="1:10" s="12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A28" s="10" t="s">
         <v>29</v>
       </c>
@@ -1591,12 +1487,8 @@
       <c r="J28" s="14">
         <v>11.950000000000003</v>
       </c>
-      <c r="K28" s="14">
-        <f t="shared" si="0"/>
-        <v>11.947484009267001</v>
-      </c>
-    </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.3">
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A29" s="4" t="s">
         <v>30</v>
       </c>
@@ -1627,12 +1519,8 @@
       <c r="J29" s="14">
         <v>123.37</v>
       </c>
-      <c r="K29" s="14">
-        <f t="shared" si="0"/>
-        <v>123.36330897725999</v>
-      </c>
-    </row>
-    <row r="30" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="30" spans="1:10" s="12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A30" s="10" t="s">
         <v>31</v>
       </c>
@@ -1663,12 +1551,8 @@
       <c r="J30" s="14">
         <v>10.119999999999999</v>
       </c>
-      <c r="K30" s="14">
-        <f t="shared" si="0"/>
-        <v>10.115446615326681</v>
-      </c>
-    </row>
-    <row r="31" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="31" spans="1:10" s="12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A31" s="10" t="s">
         <v>32</v>
       </c>
@@ -1699,12 +1583,8 @@
       <c r="J31" s="14">
         <v>13.68</v>
       </c>
-      <c r="K31" s="14">
-        <f t="shared" si="0"/>
-        <v>13.678158084240003</v>
-      </c>
-    </row>
-    <row r="32" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="32" spans="1:10" s="12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B32" s="13"/>
       <c r="C32" s="13"/>
     </row>
@@ -1720,15 +1600,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101008990E4295803CF4CB9A93C357F2BD71E" ma:contentTypeVersion="10" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="3f8fd23b4e99e28017c9d094d0d91850">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="1c50504a-f263-42ab-a44b-81a94ffe0954" xmlns:ns3="139635ce-1ed1-4d40-af19-24de1d62ba3e" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="9001ed0c4d841bceb748452573bbf4a9" ns2:_="" ns3:_="">
     <xsd:import namespace="1c50504a-f263-42ab-a44b-81a94ffe0954"/>
@@ -1933,6 +1804,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DE1DCAA5-E065-4E1E-98F9-8377A52119A3}">
   <ds:schemaRefs>
@@ -1943,14 +1823,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B1612B5D-BE83-4992-9F97-7E57AEF5C74D}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{241A15A9-F376-42CD-A780-B199667CAC86}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1967,4 +1839,12 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B1612B5D-BE83-4992-9F97-7E57AEF5C74D}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>